<commit_message>
Einarbeiten Input von PL Eckerle, Start der Anforderungs-Versionisierung
</commit_message>
<xml_diff>
--- a/Projektdokumentation/Leistungsnachweis_Gasenzer/Anforderungen.xlsx
+++ b/Projektdokumentation/Leistungsnachweis_Gasenzer/Anforderungen.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
     <sheet name="Detail" sheetId="2" r:id="rId2"/>
+    <sheet name="Archiv" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -23,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="92">
   <si>
     <t>Anforderungen "Project Escape"</t>
   </si>
@@ -294,11 +292,41 @@
 - Ganzzahlig gerundete Gesamtpunktzahl 50%-84%: Neutrales Ende.
 - Ganzzahlig gerundete Gesamtpunktzahl 85%-100%: Positives Ende.</t>
   </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Sobald der Spieler das finale Level geschafft hat, soll das System das leistungsabhängige Ende der Geschichte gemäss dem Bewertungsinex anzeigen.
+- Ganzzahlig gerundeter Bewertungsinex 0%-49%: Negatives Ende.
+- Ganzzahlig gerundeter Bewertungsinex 50%-84%: Neutrales Ende.
+- Ganzzahlig gerundeter Bewertungsinex 85%-100%: Positives Ende.</t>
+  </si>
+  <si>
+    <t>Sobald ein Level abgeschlossen ist, soll das System die dort erreichte Punktzahl (zwischen 0 und 100) zu der bisherigen Gesamtpunktzahl des Benutzers addieren und das Ergebnis zusammen mit der totalen Anzahl bisher abgeschlossener Level im Spielstand eintragen. Aus diesen beiden Werten kann dann ein Bewertungsindex errechnet werden: &lt;Bewertungsindex&gt; = &lt;Gesamtpunktzahl&gt; / &lt;Anzahl abgeschlossener Levels&gt;</t>
+  </si>
+  <si>
+    <t>Das System zeigt in der Level-Übersicht (siehe Anforderung 3) den aktuellen Bewertungsindex des Spielers (siehe Anforderung 4) oben rechts in der View in der Form „Aktuelle Bewertung: &lt;Bewertungsindex&gt;“</t>
+  </si>
+  <si>
+    <t>Folgeversion</t>
+  </si>
+  <si>
+    <t>Änderungsgrund</t>
+  </si>
+  <si>
+    <t>Besprechung mit Projektleiter Eckerle, 09,12,2016</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-407]General"/>
   </numFmts>
@@ -432,7 +460,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -441,9 +469,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -455,19 +480,24 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Ausgabe" xfId="1" builtinId="21"/>
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="1" builtinId="21"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -777,458 +807,493 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1024" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="E2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="L3" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>42648</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="L4" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>42648</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="L5" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>42676</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="L6" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <v>42676</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="L7" s="18" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <v>42676</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="L8" s="18" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>42662</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="L9" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="12">
         <v>42678</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>43</v>
       </c>
+      <c r="L10" s="18" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="12">
         <v>42678</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>43</v>
       </c>
+      <c r="L11" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="12">
         <v>42678</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="11" t="s">
         <v>43</v>
       </c>
+      <c r="L12" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>42662</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="L13" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="9">
         <v>42676</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L14" s="3"/>
+      <c r="L14" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
@@ -2242,41 +2307,43 @@
       <c r="AMI14" s="3"/>
       <c r="AMJ14" s="3"/>
     </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
         <v>42662</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="3"/>
+      <c r="L15" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -3290,41 +3357,43 @@
       <c r="AMI15" s="3"/>
       <c r="AMJ15" s="3"/>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="9">
         <v>42662</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -4338,161 +4407,164 @@
       <c r="AMI16" s="3"/>
       <c r="AMJ16" s="3"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="9">
         <v>42690</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="K17" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="L17" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+    <row r="20" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7" t="s">
+      <c r="B21" s="14"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4508,17 +4580,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1024" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -4528,8 +4600,11 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="2" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -4539,8 +4614,11 @@
       <c r="C2" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="D2" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="3" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -4550,8 +4628,11 @@
       <c r="C3" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="D3" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="4" spans="1:1024" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -4561,8 +4642,11 @@
       <c r="C4" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="D4" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="5" spans="1:1024" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -4570,10 +4654,13 @@
         <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>87</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -4581,10 +4668,13 @@
         <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -4594,8 +4684,11 @@
       <c r="C7" s="2" t="s">
         <v>74</v>
       </c>
+      <c r="D7" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="8" spans="1:1024" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1024" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -4605,8 +4698,11 @@
       <c r="C8" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="D8" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -4616,8 +4712,11 @@
       <c r="C9" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="D9" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="10" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1024" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -4627,8 +4726,11 @@
       <c r="C10" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="D10" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="11" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1024" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -4638,8 +4740,11 @@
       <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="D11" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="12" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1024" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>64</v>
       </c>
@@ -4647,9 +4752,11 @@
         <v>45</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>85</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -5671,7 +5778,7 @@
       <c r="AMI12" s="3"/>
       <c r="AMJ12" s="3"/>
     </row>
-    <row r="13" spans="1:1024" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1024" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>65</v>
       </c>
@@ -5681,7 +5788,9 @@
       <c r="C13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -6703,7 +6812,7 @@
       <c r="AMI13" s="3"/>
       <c r="AMJ13" s="3"/>
     </row>
-    <row r="14" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1024" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>66</v>
       </c>
@@ -6713,7 +6822,9 @@
       <c r="C14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -7735,7 +7846,7 @@
       <c r="AMI14" s="3"/>
       <c r="AMJ14" s="3"/>
     </row>
-    <row r="15" spans="1:1024" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1024" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>76</v>
       </c>
@@ -7745,7 +7856,9 @@
       <c r="C15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -8767,13 +8880,120 @@
       <c r="AMI15" s="3"/>
       <c r="AMJ15" s="3"/>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>